<commit_message>
add discount in invoice module and report
</commit_message>
<xml_diff>
--- a/application/third_party/template/invoice.xlsx
+++ b/application/third_party/template/invoice.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\pos\application\third_party\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pos\application\third_party\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>DETAILER GALLERY</t>
   </si>
   <si>
-    <t>Jl. Kebun Raya 2 No. 14, Duri Kepa</t>
-  </si>
-  <si>
-    <t>Telp : 021-35857586</t>
-  </si>
-  <si>
-    <t>Mobile : 081808171007</t>
-  </si>
-  <si>
     <t>INVOICE</t>
   </si>
   <si>
@@ -87,6 +78,12 @@
   </si>
   <si>
     <t>(                                               )</t>
+  </si>
+  <si>
+    <t>Bill To.</t>
+  </si>
+  <si>
+    <t>Discount</t>
   </si>
 </sst>
 </file>
@@ -208,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -221,9 +218,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -267,17 +261,24 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,10 +646,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:Z17"/>
+  <dimension ref="A3:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,168 +672,182 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E6" s="18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19" t="s">
+      <c r="C9" s="29"/>
+      <c r="D9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="19"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="19"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="26" t="s">
+      <c r="F9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="22">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="22">
+      <c r="E10" s="7"/>
+      <c r="F10" s="21">
         <v>0</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="22">
+      <c r="A11" s="5"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="21">
         <v>0</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="23">
-        <f>SUM(F9:F11)</f>
+      <c r="A12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="21">
         <v>0</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G13" s="7"/>
+      <c r="A13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
+      <c r="A14" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="22">
+        <f>SUM(F10:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A13:E13"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>

</xml_diff>